<commit_message>
Small changes to uml
</commit_message>
<xml_diff>
--- a/Documentation/Product Backlog.xlsx
+++ b/Documentation/Product Backlog.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Morgan\Documents\Aberystwyth University\Year 5\repo\Documentation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B34A197B-3EF4-4C9F-9526-6B4288799AEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="94">
   <si>
     <t>Task/Functionality</t>
   </si>
@@ -292,12 +298,18 @@
   </si>
   <si>
     <t>1 hour</t>
+  </si>
+  <si>
+    <t>Write Test Plan</t>
+  </si>
+  <si>
+    <t>Write Solr Report</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -433,7 +445,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -441,6 +453,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -489,7 +504,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -522,9 +537,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -557,6 +589,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -732,11 +781,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C5:G59"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="C5:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -870,87 +919,83 @@
     </row>
     <row r="13" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>16</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="D13" s="5"/>
       <c r="E13" s="5"/>
-      <c r="F13" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
     </row>
     <row r="14" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="D14" s="5"/>
       <c r="E14" s="5"/>
-      <c r="F14" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
     </row>
     <row r="15" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="5">
+        <v>7</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="5">
+        <v>10</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D17" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="3:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="1" t="s">
+      <c r="E17" s="5">
+        <v>11</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="3:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="3:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="5"/>
+      <c r="E18" s="5">
+        <v>8</v>
+      </c>
       <c r="F18" s="5" t="s">
         <v>17</v>
       </c>
@@ -958,14 +1003,16 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C19" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E19" s="5"/>
+        <v>23</v>
+      </c>
+      <c r="E19" s="5">
+        <v>9</v>
+      </c>
       <c r="F19" s="5" t="s">
         <v>17</v>
       </c>
@@ -973,14 +1020,16 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C20" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E20" s="5"/>
+        <v>23</v>
+      </c>
+      <c r="E20" s="5">
+        <v>12</v>
+      </c>
       <c r="F20" s="5" t="s">
         <v>17</v>
       </c>
@@ -990,10 +1039,10 @@
     </row>
     <row r="21" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C21" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5" t="s">
@@ -1003,12 +1052,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="3:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C22" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5" t="s">
@@ -1018,9 +1067,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="3:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C23" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>31</v>
@@ -1033,9 +1082,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="3:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C24" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>31</v>
@@ -1048,12 +1097,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C25" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="5" t="s">
@@ -1065,10 +1114,10 @@
     </row>
     <row r="26" spans="3:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C26" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="5" t="s">
@@ -1080,10 +1129,10 @@
     </row>
     <row r="27" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C27" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="5" t="s">
@@ -1093,9 +1142,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C28" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>36</v>
@@ -1108,12 +1157,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="3:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C29" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E29" s="5"/>
       <c r="F29" s="5" t="s">
@@ -1123,12 +1172,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="3:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C30" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="5" t="s">
@@ -1138,12 +1187,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="3:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C31" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E31" s="5"/>
       <c r="F31" s="5" t="s">
@@ -1153,12 +1202,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C32" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E32" s="5"/>
       <c r="F32" s="5" t="s">
@@ -1168,12 +1217,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="3:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C33" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E33" s="5"/>
       <c r="F33" s="5" t="s">
@@ -1183,12 +1232,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="3:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C34" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="5" t="s">
@@ -1200,29 +1249,29 @@
     </row>
     <row r="35" spans="3:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C35" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="5" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="3:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C36" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="E36" s="5"/>
       <c r="F36" s="5" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="G36" s="5" t="s">
         <v>18</v>
@@ -1230,10 +1279,10 @@
     </row>
     <row r="37" spans="3:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C37" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E37" s="5"/>
       <c r="F37" s="5" t="s">
@@ -1245,10 +1294,10 @@
     </row>
     <row r="38" spans="3:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C38" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="E38" s="5"/>
       <c r="F38" s="5" t="s">
@@ -1260,10 +1309,10 @@
     </row>
     <row r="39" spans="3:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C39" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E39" s="5"/>
       <c r="F39" s="5" t="s">
@@ -1275,10 +1324,10 @@
     </row>
     <row r="40" spans="3:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C40" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E40" s="5"/>
       <c r="F40" s="5" t="s">
@@ -1288,12 +1337,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C41" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E41" s="5"/>
       <c r="F41" s="5" t="s">
@@ -1303,12 +1352,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C42" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E42" s="5"/>
       <c r="F42" s="5" t="s">
@@ -1318,16 +1367,16 @@
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="3:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C43" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>20</v>
+        <v>62</v>
       </c>
       <c r="E43" s="5"/>
       <c r="F43" s="5" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="G43" s="5" t="s">
         <v>18</v>
@@ -1335,25 +1384,25 @@
     </row>
     <row r="44" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C44" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E44" s="5"/>
       <c r="F44" s="5" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="G44" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="45" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C45" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="E45" s="5"/>
       <c r="F45" s="5" t="s">
@@ -1363,12 +1412,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="46" spans="3:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C46" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E46" s="5"/>
       <c r="F46" s="5" t="s">
@@ -1378,12 +1427,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="3:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C47" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="E47" s="5"/>
       <c r="F47" s="5" t="s">
@@ -1393,12 +1442,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="3:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C48" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E48" s="5"/>
       <c r="F48" s="5" t="s">
@@ -1410,7 +1459,7 @@
     </row>
     <row r="49" spans="3:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C49" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D49" s="5" t="s">
         <v>72</v>
@@ -1425,7 +1474,7 @@
     </row>
     <row r="50" spans="3:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C50" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D50" s="5" t="s">
         <v>72</v>
@@ -1440,10 +1489,10 @@
     </row>
     <row r="51" spans="3:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C51" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E51" s="5"/>
       <c r="F51" s="5" t="s">
@@ -1453,12 +1502,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="52" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C52" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="E52" s="5"/>
       <c r="F52" s="5" t="s">
@@ -1468,12 +1517,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="53" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C53" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E53" s="5"/>
       <c r="F53" s="5" t="s">
@@ -1485,7 +1534,7 @@
     </row>
     <row r="54" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C54" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D54" s="5" t="s">
         <v>79</v>
@@ -1498,12 +1547,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="55" spans="3:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C55" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E55" s="5"/>
       <c r="F55" s="5" t="s">
@@ -1515,14 +1564,14 @@
     </row>
     <row r="56" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C56" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>16</v>
+        <v>79</v>
       </c>
       <c r="E56" s="5"/>
       <c r="F56" s="5" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="G56" s="5" t="s">
         <v>18</v>
@@ -1530,25 +1579,25 @@
     </row>
     <row r="57" spans="3:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C57" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="E57" s="5"/>
       <c r="F57" s="5" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="G57" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="58" spans="3:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C58" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="E58" s="5"/>
       <c r="F58" s="5" t="s">
@@ -1558,18 +1607,48 @@
         <v>18</v>
       </c>
     </row>
-    <row r="59" spans="3:7" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="3:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C59" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>77</v>
+        <v>23</v>
       </c>
       <c r="E59" s="5"/>
       <c r="F59" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="G59" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="60" spans="3:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C60" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E60" s="5"/>
+      <c r="F60" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="G60" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="61" spans="3:7" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C61" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E61" s="5"/>
+      <c r="F61" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="G59" s="5" t="s">
+      <c r="G61" s="5" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1580,7 +1659,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1592,7 +1671,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Added ideas to API design
</commit_message>
<xml_diff>
--- a/Documentation/Product Backlog.xlsx
+++ b/Documentation/Product Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Morgan\Documents\Aberystwyth University\Year 5\repo\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B58141E-855D-49A7-9F49-32254EFA2C17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F5DBA21-4DDE-49C6-BB3D-5382EE8D0E28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -125,9 +125,6 @@
     <t>‘Deleted’ messages are not shown to users</t>
   </si>
   <si>
-    <t>Basic Module Entity/Content</t>
-  </si>
-  <si>
     <t>MR-FR1</t>
   </si>
   <si>
@@ -353,10 +350,13 @@
     <t>Message Entiy Content (From DB tables)</t>
   </si>
   <si>
-    <t>Code</t>
-  </si>
-  <si>
     <t>Category</t>
+  </si>
+  <si>
+    <t>Implementation</t>
+  </si>
+  <si>
+    <t>Module Entity/Content (From DB Tables)</t>
   </si>
 </sst>
 </file>
@@ -989,8 +989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C5:N66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1007,13 +1007,13 @@
     <row r="5" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="3:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>0</v>
@@ -1030,16 +1030,16 @@
         <v>5</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F7" s="3">
         <v>1</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>6</v>
@@ -1050,16 +1050,16 @@
         <v>7</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F8" s="6">
         <v>2</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H8" s="7" t="s">
         <v>8</v>
@@ -1067,42 +1067,42 @@
     </row>
     <row r="9" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C9" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F9" s="6">
         <v>3</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C10" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F10" s="14">
         <v>4</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="3:8" x14ac:dyDescent="0.25">
@@ -1110,16 +1110,16 @@
         <v>3</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F11" s="6">
         <v>5</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H11" s="7" t="s">
         <v>4</v>
@@ -1130,16 +1130,16 @@
         <v>9</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F12" s="6">
         <v>6</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H12" s="7" t="s">
         <v>4</v>
@@ -1150,16 +1150,16 @@
         <v>10</v>
       </c>
       <c r="D13" s="24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F13" s="6">
         <v>7</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H13" s="7" t="s">
         <v>11</v>
@@ -1167,62 +1167,62 @@
     </row>
     <row r="14" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C14" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D14" s="24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F14" s="6">
         <v>8</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C15" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F15" s="6">
         <v>9</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F16" s="14">
         <v>10</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="3:14" x14ac:dyDescent="0.25">
@@ -1245,7 +1245,7 @@
     </row>
     <row r="18" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C18" s="27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D18" s="24" t="s">
         <v>107</v>
@@ -1345,17 +1345,17 @@
     </row>
     <row r="23" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C23" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D23" s="24" t="s">
         <v>107</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F23" s="6"/>
       <c r="G23" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H23" s="7" t="s">
         <v>14</v>
@@ -1363,7 +1363,7 @@
     </row>
     <row r="24" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C24" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D24" s="24" t="s">
         <v>107</v>
@@ -1373,7 +1373,7 @@
       </c>
       <c r="F24" s="6"/>
       <c r="G24" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H24" s="7" t="s">
         <v>14</v>
@@ -1381,7 +1381,7 @@
     </row>
     <row r="25" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C25" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D25" s="24" t="s">
         <v>107</v>
@@ -1391,7 +1391,7 @@
       </c>
       <c r="F25" s="6"/>
       <c r="G25" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H25" s="7" t="s">
         <v>14</v>
@@ -1399,7 +1399,7 @@
     </row>
     <row r="26" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C26" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D26" s="24" t="s">
         <v>107</v>
@@ -1409,7 +1409,7 @@
       </c>
       <c r="F26" s="6"/>
       <c r="G26" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H26" s="7" t="s">
         <v>14</v>
@@ -1417,7 +1417,7 @@
     </row>
     <row r="27" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C27" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D27" s="24" t="s">
         <v>107</v>
@@ -1427,7 +1427,7 @@
       </c>
       <c r="F27" s="6"/>
       <c r="G27" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H27" s="7" t="s">
         <v>14</v>
@@ -1435,7 +1435,7 @@
     </row>
     <row r="28" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C28" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D28" s="24" t="s">
         <v>107</v>
@@ -1445,7 +1445,7 @@
       </c>
       <c r="F28" s="6"/>
       <c r="G28" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H28" s="7" t="s">
         <v>14</v>
@@ -1453,13 +1453,13 @@
     </row>
     <row r="29" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C29" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D29" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F29" s="6"/>
       <c r="G29" s="14" t="s">
@@ -1471,13 +1471,13 @@
     </row>
     <row r="30" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C30" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D30" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E30" s="14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F30" s="6"/>
       <c r="G30" s="14" t="s">
@@ -1489,11 +1489,11 @@
     </row>
     <row r="31" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C31" s="2" t="s">
-        <v>31</v>
+        <v>108</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F31" s="3">
         <v>1</v>
@@ -1507,11 +1507,11 @@
     </row>
     <row r="32" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C32" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D32" s="6"/>
       <c r="E32" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F32" s="6">
         <v>2</v>
@@ -1525,11 +1525,11 @@
     </row>
     <row r="33" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C33" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D33" s="6"/>
       <c r="E33" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F33" s="6">
         <v>3</v>
@@ -1543,11 +1543,11 @@
     </row>
     <row r="34" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C34" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D34" s="6"/>
       <c r="E34" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F34" s="14">
         <v>5</v>
@@ -1561,11 +1561,11 @@
     </row>
     <row r="35" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C35" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D35" s="6"/>
       <c r="E35" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F35" s="14">
         <v>4</v>
@@ -1579,11 +1579,11 @@
     </row>
     <row r="36" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C36" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D36" s="6"/>
       <c r="E36" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F36" s="6"/>
       <c r="G36" s="6" t="s">
@@ -1595,11 +1595,11 @@
     </row>
     <row r="37" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C37" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D37" s="6"/>
       <c r="E37" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F37" s="6"/>
       <c r="G37" s="6" t="s">
@@ -1611,11 +1611,11 @@
     </row>
     <row r="38" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C38" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D38" s="16"/>
       <c r="E38" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F38" s="16">
         <v>1</v>
@@ -1629,11 +1629,11 @@
     </row>
     <row r="39" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C39" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D39" s="6"/>
       <c r="E39" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F39" s="6">
         <v>2</v>
@@ -1647,11 +1647,11 @@
     </row>
     <row r="40" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C40" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D40" s="21"/>
       <c r="E40" s="21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F40" s="21">
         <v>3</v>
@@ -1665,15 +1665,15 @@
     </row>
     <row r="41" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C41" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D41" s="16"/>
       <c r="E41" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F41" s="16"/>
       <c r="G41" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H41" s="17" t="s">
         <v>14</v>
@@ -1681,15 +1681,15 @@
     </row>
     <row r="42" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C42" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D42" s="6"/>
       <c r="E42" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F42" s="6"/>
       <c r="G42" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H42" s="19" t="s">
         <v>14</v>
@@ -1697,15 +1697,15 @@
     </row>
     <row r="43" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C43" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D43" s="6"/>
       <c r="E43" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F43" s="6"/>
       <c r="G43" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H43" s="19" t="s">
         <v>14</v>
@@ -1713,7 +1713,7 @@
     </row>
     <row r="44" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C44" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D44" s="6"/>
       <c r="E44" s="6" t="s">
@@ -1721,7 +1721,7 @@
       </c>
       <c r="F44" s="6"/>
       <c r="G44" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H44" s="19" t="s">
         <v>14</v>
@@ -1729,11 +1729,11 @@
     </row>
     <row r="45" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C45" s="26" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D45" s="6"/>
       <c r="E45" s="14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F45" s="6"/>
       <c r="G45" s="6" t="s">
@@ -1851,17 +1851,17 @@
     </row>
     <row r="52" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C52" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D52" s="16"/>
       <c r="E52" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F52" s="16">
         <v>1</v>
       </c>
       <c r="G52" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H52" s="17" t="s">
         <v>14</v>
@@ -1869,17 +1869,17 @@
     </row>
     <row r="53" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C53" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D53" s="21"/>
       <c r="E53" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F53" s="21">
         <v>2</v>
       </c>
       <c r="G53" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H53" s="22" t="s">
         <v>14</v>
@@ -1887,15 +1887,15 @@
     </row>
     <row r="54" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C54" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D54" s="6"/>
       <c r="E54" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F54" s="6"/>
       <c r="G54" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H54" s="7" t="s">
         <v>14</v>
@@ -1903,15 +1903,15 @@
     </row>
     <row r="55" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C55" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D55" s="6"/>
       <c r="E55" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F55" s="6"/>
       <c r="G55" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H55" s="7" t="s">
         <v>14</v>
@@ -1919,15 +1919,15 @@
     </row>
     <row r="56" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C56" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D56" s="6"/>
       <c r="E56" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F56" s="6"/>
       <c r="G56" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H56" s="7" t="s">
         <v>14</v>
@@ -1935,15 +1935,15 @@
     </row>
     <row r="57" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C57" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D57" s="6"/>
       <c r="E57" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F57" s="6"/>
       <c r="G57" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H57" s="7" t="s">
         <v>14</v>
@@ -1951,15 +1951,15 @@
     </row>
     <row r="58" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C58" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D58" s="6"/>
       <c r="E58" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F58" s="6"/>
       <c r="G58" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H58" s="7" t="s">
         <v>14</v>
@@ -1967,15 +1967,15 @@
     </row>
     <row r="59" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C59" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D59" s="9"/>
       <c r="E59" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F59" s="9"/>
       <c r="G59" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H59" s="10" t="s">
         <v>14</v>
@@ -1983,15 +1983,15 @@
     </row>
     <row r="60" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C60" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D60" s="3"/>
       <c r="E60" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F60" s="3"/>
       <c r="G60" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H60" s="4" t="s">
         <v>14</v>
@@ -1999,15 +1999,15 @@
     </row>
     <row r="61" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C61" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D61" s="6"/>
       <c r="E61" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F61" s="6"/>
       <c r="G61" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H61" s="7" t="s">
         <v>14</v>
@@ -2015,15 +2015,15 @@
     </row>
     <row r="62" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C62" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D62" s="6"/>
       <c r="E62" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F62" s="6"/>
       <c r="G62" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H62" s="7" t="s">
         <v>14</v>
@@ -2031,15 +2031,15 @@
     </row>
     <row r="63" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C63" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D63" s="6"/>
       <c r="E63" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F63" s="6"/>
       <c r="G63" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H63" s="7" t="s">
         <v>14</v>
@@ -2047,15 +2047,15 @@
     </row>
     <row r="64" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C64" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D64" s="6"/>
       <c r="E64" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F64" s="6"/>
       <c r="G64" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H64" s="7" t="s">
         <v>14</v>
@@ -2063,15 +2063,15 @@
     </row>
     <row r="65" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C65" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D65" s="6"/>
       <c r="E65" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F65" s="6"/>
       <c r="G65" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H65" s="7" t="s">
         <v>14</v>
@@ -2079,15 +2079,15 @@
     </row>
     <row r="66" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C66" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D66" s="9"/>
       <c r="E66" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F66" s="9"/>
       <c r="G66" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H66" s="10" t="s">
         <v>14</v>

</xml_diff>